<commit_message>
WIP: importing DHIS2 categories in custom models
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18120"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://logicaloutcomes.sharepoint.com/sites/sis-mci-17/Shared Documents/CCSD Data/A) REQUIREMENTS/INDICATORS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafen/.virtualenvs/indicatorregistry/src/aristotle-indicators/indicators/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="841" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34220" yWindow="-16660" windowWidth="25600" windowHeight="15460" tabRatio="841" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -26,9 +26,15 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Data Elements'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Indicators!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="146">
   <si>
     <t>Indicator name</t>
   </si>
@@ -280,15 +286,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>Category option name</t>
-  </si>
-  <si>
-    <t>Category name</t>
-  </si>
-  <si>
-    <t>Category Combination</t>
   </si>
   <si>
     <t>OptionSetName</t>
@@ -579,12 +576,39 @@
   <si>
     <t>Georgi</t>
   </si>
+  <si>
+    <t>SexCat</t>
+  </si>
+  <si>
+    <t>Category Option Code</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>Category Code</t>
+  </si>
+  <si>
+    <t>Sex Category</t>
+  </si>
+  <si>
+    <t>YesNoDK</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>I don't know</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,11 +829,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent3 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1113,42 +1137,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="159" zoomScaleNormal="159" zoomScalePageLayoutView="159" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="12" customWidth="1"/>
-    <col min="6" max="7" width="35.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="59.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="63.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" style="12" customWidth="1"/>
+    <col min="6" max="7" width="35.83203125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="12" customWidth="1"/>
+    <col min="10" max="10" width="59.1640625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="22.5" style="12" customWidth="1"/>
     <col min="12" max="13" width="25" style="12" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" style="12" customWidth="1"/>
     <col min="16" max="16" width="24" style="12" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="12"/>
-    <col min="18" max="18" width="23.7109375" style="12" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="12"/>
+    <col min="18" max="18" width="23.6640625" style="12" customWidth="1"/>
     <col min="19" max="19" width="20" style="12" customWidth="1"/>
-    <col min="20" max="16384" width="17.28515625" style="12"/>
+    <col min="20" max="16384" width="17.33203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" ht="47.25" customHeight="1">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="13" customFormat="1" ht="27" customHeight="1">
+    <row r="2" spans="1:21" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
@@ -1275,7 +1299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="60">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1326,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="71.25" customHeight="1">
+    <row r="4" spans="1:21" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -1344,33 +1368,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="51.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="4" max="5" width="18.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="22" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="20.140625" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="17.28515625" style="5"/>
+    <col min="8" max="8" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="20.1640625" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="17.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="24" customHeight="1">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
@@ -1417,7 +1441,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" ht="15">
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>66</v>
       </c>
@@ -1446,7 +1470,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1474,7 +1498,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1507,7 +1531,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
@@ -1550,19 +1574,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1">
+    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>52</v>
       </c>
@@ -1576,7 +1600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1587,7 +1611,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1605,45 +1629,64 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1652,33 +1695,54 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="20" customFormat="1">
+    <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
         <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1687,33 +1751,92 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>88</v>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1722,543 +1845,543 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="18" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="18" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="18" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="21" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="18"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="18"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="18"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="18"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="20" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="19"/>
+    </row>
+    <row r="29" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row r="30" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="23" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="19"/>
-    </row>
-    <row r="29" spans="1:1" s="19" customFormat="1">
-      <c r="A29" s="19" t="s">
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="19" customFormat="1"/>
-    <row r="31" spans="1:1" s="19" customFormat="1"/>
-    <row r="32" spans="1:1" s="19" customFormat="1"/>
-    <row r="33" spans="1:1" s="19" customFormat="1"/>
-    <row r="34" spans="1:1">
-      <c r="A34" s="20" t="s">
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="24"/>
+    </row>
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="25"/>
+    </row>
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75">
-      <c r="A41" s="24" t="s">
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75">
-      <c r="A42" s="24"/>
-    </row>
-    <row r="43" spans="1:1" ht="15.75">
-      <c r="A43" s="24" t="s">
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="25"/>
-    </row>
-    <row r="45" spans="1:1" ht="15.75">
-      <c r="A45" s="26" t="s">
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="24"/>
+    </row>
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75">
-      <c r="A46" s="26" t="s">
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="24"/>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="24" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15.75">
-      <c r="A47" s="24" t="s">
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="24"/>
+    </row>
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="24" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15.75">
-      <c r="A48" s="24"/>
-    </row>
-    <row r="49" spans="1:1" ht="15.75">
-      <c r="A49" s="24" t="s">
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+    </row>
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15.75">
-      <c r="A50" s="24"/>
-    </row>
-    <row r="51" spans="1:1" ht="15.75">
-      <c r="A51" s="24" t="s">
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="24"/>
+    </row>
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.75">
-      <c r="A52" s="24"/>
-    </row>
-    <row r="53" spans="1:1" ht="15.75">
-      <c r="A53" s="24" t="s">
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="24"/>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.75">
-      <c r="A54" s="24"/>
-    </row>
-    <row r="55" spans="1:1" ht="15.75">
-      <c r="A55" s="24" t="s">
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="24"/>
+    </row>
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="24"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15.75">
-      <c r="A56" s="24"/>
-    </row>
-    <row r="57" spans="1:1" ht="15.75">
-      <c r="A57" s="24" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.75">
-      <c r="A58" s="24"/>
-    </row>
-    <row r="59" spans="1:1" ht="15.75">
-      <c r="A59" s="24" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="28"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15.75">
-      <c r="A60" s="24"/>
-    </row>
-    <row r="61" spans="1:1" ht="15.75">
-      <c r="A61" s="24"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="27" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="28"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="28" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="28"/>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="28"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="28"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="29" t="s">
         <v>53</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D71" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="30">
         <v>3501</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D72" s="30">
         <v>33966</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="30">
         <v>3501005</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D73" s="30">
         <v>38477</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="30">
         <v>3501011</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D74" s="30">
         <v>37964</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="30">
         <v>3501012</v>
       </c>
       <c r="B75" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" s="31" t="s">
         <v>124</v>
-      </c>
-      <c r="C75" s="31" t="s">
-        <v>127</v>
       </c>
       <c r="D75" s="30">
         <v>29667</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="30">
         <v>3501020</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D76" s="30">
         <v>32716</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="30">
         <v>3501030</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D77" s="30">
         <v>39345</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="30">
         <v>3501042</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D78" s="30">
         <v>37020</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="30">
         <v>3501050</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D79" s="30">
         <v>32181</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="28"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="28"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="28"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="28"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="28"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="29" t="s">
         <v>53</v>
       </c>
       <c r="B94" s="29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="30">
         <v>3501</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D95" s="30">
         <v>91165</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="30">
         <v>3501005</v>
       </c>
       <c r="B96" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D96" s="30">
         <v>10950</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="30">
         <v>3501011</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D97" s="30">
         <v>10450</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="30">
         <v>3501012</v>
       </c>
       <c r="B98" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C98" s="31" t="s">
         <v>124</v>
-      </c>
-      <c r="C98" s="31" t="s">
-        <v>127</v>
       </c>
       <c r="D98" s="30">
         <v>37745</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="30">
         <v>3501020</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D99" s="30">
         <v>8990</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="30">
         <v>3501030</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D100" s="30">
         <v>9255</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="30">
         <v>3501042</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D101" s="30">
         <v>5440</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="30">
         <v>3501050</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D102" s="30">
         <v>8330</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="28"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="28"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="28"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="28"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="28" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A62" r:id="rId1" display="mailto:georgi@logicaloutcomes.net" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A62" r:id="rId1" display="mailto:georgi@logicaloutcomes.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2429,13 +2552,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{363B1A9A-DB3D-4928-A48D-C35095503C70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{363B1A9A-DB3D-4928-A48D-C35095503C70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a895c725-c39c-400e-9016-6feaa1a20ace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F33526A-FE36-42C7-8514-DF5833464662}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F33526A-FE36-42C7-8514-DF5833464662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3FB6AB5-B1E1-483A-8A3F-2CCCFE424BEC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3FB6AB5-B1E1-483A-8A3F-2CCCFE424BEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added DataElements to import script for DHIS2.
Also included several improvements for the DHIS2 import script
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34220" yWindow="-16660" windowWidth="25600" windowHeight="15460" tabRatio="841" activeTab="5"/>
+    <workbookView xWindow="-5480" yWindow="-18920" windowWidth="28800" windowHeight="17540" tabRatio="841" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1528,7 +1528,7 @@
         <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1559,7 +1559,7 @@
         <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1699,7 +1699,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1762,7 +1762,7 @@
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
Added filters and templates to browse indicators
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5480" yWindow="-18920" windowWidth="28800" windowHeight="17540" tabRatio="841" activeTab="5"/>
+    <workbookView xWindow="2520" yWindow="-19100" windowWidth="28800" windowHeight="17540" tabRatio="841"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="142">
   <si>
     <t>Indicator name</t>
   </si>
@@ -53,10 +53,6 @@
     <t>Short name length</t>
   </si>
   <si>
-    <t xml:space="preserve">Indicator code
-</t>
-  </si>
-  <si>
     <t>Indicator question text</t>
   </si>
   <si>
@@ -90,26 +86,9 @@
     <t>Rationale for selection</t>
   </si>
   <si>
-    <t xml:space="preserve">Terms of use
-</t>
-  </si>
-  <si>
     <t>TAGS: Languages</t>
   </si>
   <si>
-    <t>TAGS: Theory of change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGS: Data collection 
-</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>SubDomain</t>
-  </si>
-  <si>
     <t>Full name of indicator</t>
   </si>
   <si>
@@ -156,19 +135,6 @@
   </si>
   <si>
     <t>The languages available for the data collection instrument</t>
-  </si>
-  <si>
-    <t>Choices: Impact; Organizational practices; behaviour; Knowledge and attitudes; Experience; Reach; Activities; Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choices: Administrative data; Public dataset; Participant survey; Service provider survey; Community survey; Observation
-</t>
-  </si>
-  <si>
-    <t>Indicator group set</t>
-  </si>
-  <si>
-    <t>Indicator group</t>
   </si>
   <si>
     <t>Average employment earnings of [Type of newcomer*] applicants relative as a percentage of the Canadian [or community or provincial] average, five years after landing</t>
@@ -603,12 +569,30 @@
   <si>
     <t>I don't know</t>
   </si>
+  <si>
+    <t>Indicator code</t>
+  </si>
+  <si>
+    <t>Numerator description</t>
+  </si>
+  <si>
+    <t>Numerator computation</t>
+  </si>
+  <si>
+    <t>Denominator description</t>
+  </si>
+  <si>
+    <t>Denominator computation</t>
+  </si>
+  <si>
+    <t>Terms of use</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,8 +679,37 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -721,6 +734,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -738,7 +763,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -767,23 +792,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -799,9 +812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -825,6 +835,33 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,17 +872,7 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1143,225 +1170,236 @@
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" zoomScalePageLayoutView="159" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" zoomScalePageLayoutView="159" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" style="12" customWidth="1"/>
-    <col min="6" max="7" width="35.83203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="12" customWidth="1"/>
-    <col min="10" max="10" width="59.1640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="22.5" style="12" customWidth="1"/>
-    <col min="12" max="13" width="25" style="12" customWidth="1"/>
-    <col min="14" max="14" width="25.33203125" style="12" customWidth="1"/>
-    <col min="15" max="15" width="26.6640625" style="12" customWidth="1"/>
-    <col min="16" max="16" width="24" style="12" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" style="12"/>
-    <col min="18" max="18" width="23.6640625" style="12" customWidth="1"/>
-    <col min="19" max="19" width="20" style="12" customWidth="1"/>
-    <col min="20" max="16384" width="17.33203125" style="12"/>
+    <col min="1" max="1" width="63.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" style="10" customWidth="1"/>
+    <col min="6" max="7" width="35.83203125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="10" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="10" customWidth="1"/>
+    <col min="10" max="10" width="59.1640625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="22.5" style="10" customWidth="1"/>
+    <col min="12" max="13" width="25" style="10" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="24" style="10" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="10"/>
+    <col min="18" max="18" width="23.6640625" style="10" customWidth="1"/>
+    <col min="19" max="19" width="20" style="10" customWidth="1"/>
+    <col min="20" max="16384" width="17.33203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="L1" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="O1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="P1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="Q1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="R1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="S1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="T1" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:21" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="B2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="C2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="D2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="E2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="F2" s="29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="O2" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="P2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="Q2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="R2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="S2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="T2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="U2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:21" ht="120" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="B3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="33">
+        <v>165</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="13" t="s">
+    </row>
+    <row r="4" spans="1:21" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="B4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="33">
+        <v>132</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="13" t="s">
+      <c r="H4" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="16">
-        <f>LEN(B3)</f>
-        <v>165</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="16">
-        <f t="shared" ref="C4" si="0">LEN(B4)</f>
-        <v>132</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>46</v>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:C4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>50</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="21" fitToHeight="8" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -1375,7 +1413,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1396,170 +1434,170 @@
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="E2" s="7">
         <f>LEN(D2)</f>
         <v>47</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="17" t="s">
-        <v>42</v>
+      <c r="G2" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E3" s="7">
         <f>LEN(D3)</f>
         <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" ref="E4:E5" si="0">LEN(D4)</f>
         <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1577,49 +1615,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>55</v>
+    <row r="1" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1669,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1644,49 +1680,49 @@
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>138</v>
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1699,7 +1735,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1711,38 +1747,38 @@
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>140</v>
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1754,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1769,74 +1805,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>85</v>
+      <c r="A1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>123456</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>123456</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1858,525 +1894,525 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>86</v>
+      <c r="A2" s="16" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>88</v>
+      <c r="A5" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>89</v>
+      <c r="A6" s="14" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>90</v>
+      <c r="A7" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>91</v>
+      <c r="A10" s="17" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>92</v>
+      <c r="A11" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="14"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="14"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>93</v>
+      <c r="A18" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
-        <v>98</v>
+      <c r="A27" s="18" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-    </row>
-    <row r="29" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
-        <v>100</v>
+      <c r="A34" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="19"/>
+    </row>
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+    </row>
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="19"/>
+    </row>
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="19"/>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="19"/>
+    </row>
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="19"/>
+    </row>
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="19"/>
+    </row>
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="19"/>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-    </row>
-    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="19"/>
+    </row>
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="19"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-    </row>
-    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="26" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="26" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="23"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="23"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-    </row>
-    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="23"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="24" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-    </row>
-    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="24" t="s">
+      <c r="C71" s="24" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="24"/>
-    </row>
-    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="24" t="s">
+      <c r="D71" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="25">
+        <v>3501</v>
+      </c>
+      <c r="B72" s="26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-    </row>
-    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="24" t="s">
+      <c r="C72" s="26" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-    </row>
-    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="24" t="s">
+      <c r="D72" s="25">
+        <v>33966</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="25">
+        <v>3501005</v>
+      </c>
+      <c r="B73" s="26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-    </row>
-    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="24" t="s">
+      <c r="C73" s="26" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-    </row>
-    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="27" t="s">
+      <c r="D73" s="25">
+        <v>38477</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="25">
+        <v>3501011</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="26" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="28" t="s">
+      <c r="D74" s="25">
+        <v>37964</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="25">
+        <v>3501012</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="26" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="28"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
+      <c r="D75" s="25">
+        <v>29667</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="25">
+        <v>3501020</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="26" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="28"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="28" t="s">
+      <c r="D76" s="25">
+        <v>32716</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="25">
+        <v>3501030</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="26" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="28"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" s="29" t="s">
+      <c r="D77" s="25">
+        <v>39345</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="25">
+        <v>3501042</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C71" s="29" t="s">
+      <c r="D78" s="25">
+        <v>37020</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="25">
+        <v>3501050</v>
+      </c>
+      <c r="B79" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D71" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="30">
+      <c r="D79" s="25">
+        <v>32181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="23"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="23"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="23"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="23"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="23"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="25">
         <v>3501</v>
       </c>
-      <c r="B72" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D72" s="30">
-        <v>33966</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="30">
+      <c r="B95" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95" s="25">
+        <v>91165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="25">
         <v>3501005</v>
       </c>
-      <c r="B73" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D73" s="30">
-        <v>38477</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="30">
+      <c r="B96" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D96" s="25">
+        <v>10950</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="25">
         <v>3501011</v>
       </c>
-      <c r="B74" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D74" s="30">
-        <v>37964</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="30">
+      <c r="B97" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D97" s="25">
+        <v>10450</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="25">
         <v>3501012</v>
       </c>
-      <c r="B75" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="31" t="s">
+      <c r="B98" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C98" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" s="25">
+        <v>37745</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="25">
+        <v>3501020</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C99" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D99" s="25">
+        <v>8990</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="25">
+        <v>3501030</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D100" s="25">
+        <v>9255</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="25">
+        <v>3501042</v>
+      </c>
+      <c r="B101" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="25">
+        <v>5440</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="25">
+        <v>3501050</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D102" s="25">
+        <v>8330</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="23"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="23"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D75" s="30">
-        <v>29667</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="30">
-        <v>3501020</v>
-      </c>
-      <c r="B76" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="31" t="s">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="23"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D76" s="30">
-        <v>32716</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="30">
-        <v>3501030</v>
-      </c>
-      <c r="B77" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C77" s="31" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="23"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="23" t="s">
         <v>126</v>
-      </c>
-      <c r="D77" s="30">
-        <v>39345</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="30">
-        <v>3501042</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D78" s="30">
-        <v>37020</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="30">
-        <v>3501050</v>
-      </c>
-      <c r="B79" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C79" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="D79" s="30">
-        <v>32181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="28"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="28"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="28"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="28"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="28"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B94" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C94" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="D94" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="30">
-        <v>3501</v>
-      </c>
-      <c r="B95" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C95" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D95" s="30">
-        <v>91165</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="30">
-        <v>3501005</v>
-      </c>
-      <c r="B96" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C96" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D96" s="30">
-        <v>10950</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="30">
-        <v>3501011</v>
-      </c>
-      <c r="B97" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C97" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D97" s="30">
-        <v>10450</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="30">
-        <v>3501012</v>
-      </c>
-      <c r="B98" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C98" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="D98" s="30">
-        <v>37745</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="30">
-        <v>3501020</v>
-      </c>
-      <c r="B99" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C99" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="D99" s="30">
-        <v>8990</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="30">
-        <v>3501030</v>
-      </c>
-      <c r="B100" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C100" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D100" s="30">
-        <v>9255</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="30">
-        <v>3501042</v>
-      </c>
-      <c r="B101" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D101" s="30">
-        <v>5440</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="30">
-        <v>3501050</v>
-      </c>
-      <c r="B102" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C102" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="D102" s="30">
-        <v>8330</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="28"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="28"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="28"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="28"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="28" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import to DHIS2 script now uses code as main identifiers
It also add a Slot Collection to Indicators, DataElements and Value to have them grouped
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-20000" windowWidth="31860" windowHeight="19000" tabRatio="841" activeTab="5"/>
+    <workbookView xWindow="-180" yWindow="-20000" windowWidth="31860" windowHeight="19000" tabRatio="841"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
   <si>
     <t>Indicator name</t>
   </si>
@@ -951,6 +951,21 @@
   </si>
   <si>
     <t>Georgi</t>
+  </si>
+  <si>
+    <t>OCASI_0001</t>
+  </si>
+  <si>
+    <t>OCASI_0002</t>
+  </si>
+  <si>
+    <t>OCASI_0003</t>
+  </si>
+  <si>
+    <t>OCASI_0004</t>
+  </si>
+  <si>
+    <t>OCASI_0005</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1120,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1217,6 +1232,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent3 2" xfId="2"/>
@@ -1554,11 +1572,11 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1736,6 +1754,9 @@
         <f>LEN(B3)</f>
         <v>47</v>
       </c>
+      <c r="D3" s="41" t="s">
+        <v>260</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>47</v>
       </c>
@@ -1786,6 +1807,9 @@
         <f t="shared" ref="C4:C5" si="0">LEN(B4)</f>
         <v>49</v>
       </c>
+      <c r="D4" s="41" t="s">
+        <v>261</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>61</v>
       </c>
@@ -1836,6 +1860,9 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
+      <c r="D5" s="41" t="s">
+        <v>262</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>69</v>
       </c>
@@ -1886,7 +1913,9 @@
         <f t="shared" ref="C6:C7" si="1">LEN(B6)</f>
         <v>44</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="41" t="s">
+        <v>263</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>77</v>
       </c>
@@ -1939,7 +1968,9 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="41" t="s">
+        <v>264</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>88</v>
       </c>
@@ -2820,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified filters presentation and using Outcomes and categories in ind table
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -118,12 +118,6 @@
 </t>
   </si>
   <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>SubDomain</t>
-  </si>
-  <si>
     <t>Full name of indicator</t>
   </si>
   <si>
@@ -966,6 +960,12 @@
   </si>
   <si>
     <t>OCASI_0005</t>
+  </si>
+  <si>
+    <t>Outcomes</t>
+  </si>
+  <si>
+    <t>Sustainable development goals</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1573,10 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1675,333 +1675,333 @@
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>23</v>
+        <v>264</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>24</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="9">
         <f>LEN(B3)</f>
         <v>47</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="J3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="K3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="L3" s="27" t="s">
         <v>52</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>54</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="Q3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ref="C4:C5" si="0">LEN(B4)</f>
         <v>49</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="J4" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="L4" s="27" t="s">
         <v>64</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>66</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="Q4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="I5" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="26" t="s">
+      <c r="J5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="L5" s="27" t="s">
         <v>72</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>74</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="Q5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="W5" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="39">
         <f t="shared" ref="C6:C7" si="1">LEN(B6)</f>
         <v>44</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="L6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="27" t="s">
         <v>83</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="27" t="s">
-        <v>85</v>
       </c>
       <c r="N6" s="14"/>
       <c r="Q6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="W6" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="V6" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="W6" s="28" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="28" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="39">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="K7" s="14"/>
       <c r="M7" s="14"/>
       <c r="Q7" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="U7" s="14" t="s">
+      <c r="W7" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="V7" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="W7" s="28" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2032,15 +2032,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2091,66 +2091,66 @@
   <sheetData>
     <row r="1" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="E2" s="32">
         <f>LEN(D2)</f>
@@ -2158,416 +2158,416 @@
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="O2" s="23"/>
     </row>
     <row r="3" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="E3" s="32">
         <f>LEN(D3)</f>
         <v>37</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="E4" s="32">
         <f t="shared" ref="E4:E7" si="0">LEN(D4)</f>
         <v>46</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="E5" s="32">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="E6" s="32">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="E7" s="32">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="D8" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="E8" s="32">
         <f t="shared" ref="E8:E14" si="1">LEN(D8)</f>
         <v>31</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J8" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" t="s">
         <v>133</v>
-      </c>
-      <c r="K8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="D9" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="E9" s="32">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J9" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" t="s">
         <v>133</v>
-      </c>
-      <c r="K9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L9" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="D10" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="E10" s="32">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J10" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L10" t="s">
         <v>133</v>
-      </c>
-      <c r="K10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L10" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="E11" s="32">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J11" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" t="s">
         <v>133</v>
-      </c>
-      <c r="K11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E12" s="32">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J12" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" t="s">
         <v>133</v>
-      </c>
-      <c r="K12" t="s">
-        <v>134</v>
-      </c>
-      <c r="L12" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="36" t="s">
         <v>153</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>155</v>
       </c>
       <c r="E13" s="32">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J13" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" t="s">
         <v>133</v>
-      </c>
-      <c r="K13" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="36" t="s">
         <v>158</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="E14" s="32">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J14" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" t="s">
+        <v>132</v>
+      </c>
+      <c r="L14" t="s">
         <v>133</v>
-      </c>
-      <c r="K14" t="s">
-        <v>134</v>
-      </c>
-      <c r="L14" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2600,100 +2600,100 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2722,124 +2722,124 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>94</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" t="s">
-        <v>178</v>
-      </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
         <v>176</v>
       </c>
-      <c r="B3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" t="s">
-        <v>178</v>
-      </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" t="s">
         <v>179</v>
       </c>
-      <c r="B4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>181</v>
-      </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
         <v>179</v>
       </c>
-      <c r="B5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" t="s">
-        <v>181</v>
-      </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" t="s">
         <v>179</v>
       </c>
-      <c r="B6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" t="s">
-        <v>181</v>
-      </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
         <v>179</v>
       </c>
-      <c r="B7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" t="s">
-        <v>181</v>
-      </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2866,90 +2866,90 @@
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>94</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s">
         <v>176</v>
-      </c>
-      <c r="B2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" t="s">
         <v>179</v>
-      </c>
-      <c r="B3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2977,73 +2977,73 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>192</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>123456</v>
       </c>
       <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" t="s">
-        <v>197</v>
-      </c>
       <c r="F3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4">
         <v>123456</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3069,37 +3069,37 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -3107,87 +3107,87 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="37" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
     </row>
     <row r="40" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="37" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3207,17 +3207,17 @@
     <row r="42" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
     </row>
     <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -3233,17 +3233,17 @@
     </row>
     <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3251,7 +3251,7 @@
     </row>
     <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3259,7 +3259,7 @@
     </row>
     <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3267,7 +3267,7 @@
     </row>
     <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3275,7 +3275,7 @@
     </row>
     <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3283,7 +3283,7 @@
     </row>
     <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3291,7 +3291,7 @@
     </row>
     <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3302,12 +3302,12 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3315,7 +3315,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -3323,7 +3323,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3331,16 +3331,16 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3348,10 +3348,10 @@
         <v>3501</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D79" s="21">
         <v>33966</v>
@@ -3362,10 +3362,10 @@
         <v>3501005</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D80" s="21">
         <v>38477</v>
@@ -3376,10 +3376,10 @@
         <v>3501011</v>
       </c>
       <c r="B81" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" s="22" t="s">
         <v>245</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>247</v>
       </c>
       <c r="D81" s="21">
         <v>37964</v>
@@ -3390,10 +3390,10 @@
         <v>3501012</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D82" s="21">
         <v>29667</v>
@@ -3404,10 +3404,10 @@
         <v>3501020</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D83" s="21">
         <v>32716</v>
@@ -3418,10 +3418,10 @@
         <v>3501030</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D84" s="21">
         <v>39345</v>
@@ -3432,10 +3432,10 @@
         <v>3501042</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D85" s="21">
         <v>37020</v>
@@ -3446,10 +3446,10 @@
         <v>3501050</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D86" s="21">
         <v>32181</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,7 +3471,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3479,7 +3479,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3487,16 +3487,16 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3504,10 +3504,10 @@
         <v>3501</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D102" s="21">
         <v>91165</v>
@@ -3518,10 +3518,10 @@
         <v>3501005</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D103" s="21">
         <v>10950</v>
@@ -3532,10 +3532,10 @@
         <v>3501011</v>
       </c>
       <c r="B104" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C104" s="22" t="s">
         <v>245</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>247</v>
       </c>
       <c r="D104" s="21">
         <v>10450</v>
@@ -3546,10 +3546,10 @@
         <v>3501012</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D105" s="21">
         <v>37745</v>
@@ -3560,10 +3560,10 @@
         <v>3501020</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D106" s="21">
         <v>8990</v>
@@ -3574,10 +3574,10 @@
         <v>3501030</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C107" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D107" s="21">
         <v>9255</v>
@@ -3588,10 +3588,10 @@
         <v>3501042</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C108" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D108" s="21">
         <v>5440</v>
@@ -3602,10 +3602,10 @@
         <v>3501050</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C109" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D109" s="21">
         <v>8330</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
@@ -3635,7 +3635,7 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for filters and import processes
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-20000" windowWidth="31860" windowHeight="19000" tabRatio="841"/>
+    <workbookView xWindow="-180" yWindow="-20000" windowWidth="31860" windowHeight="19000" tabRatio="841" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -629,9 +629,6 @@
   </si>
   <si>
     <t>OptionUID</t>
-  </si>
-  <si>
-    <t>OptionCode</t>
   </si>
   <si>
     <t>YesNoDK</t>
@@ -966,6 +963,9 @@
   </si>
   <si>
     <t>Sustainable development goals</t>
+  </si>
+  <si>
+    <t>OptionCode (32 chars max)</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1572,7 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1675,10 +1675,10 @@
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.2">
@@ -1755,7 +1755,7 @@
         <v>47</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>45</v>
@@ -1808,7 +1808,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
@@ -1861,7 +1861,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>67</v>
@@ -1914,7 +1914,7 @@
         <v>44</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>75</v>
@@ -1969,7 +1969,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>86</v>
@@ -2961,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2992,58 +2992,58 @@
         <v>191</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>192</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
         <v>193</v>
       </c>
-      <c r="D2" t="s">
-        <v>194</v>
-      </c>
       <c r="F2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3">
         <v>123456</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <v>123456</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3069,37 +3069,37 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -3107,87 +3107,87 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
     </row>
     <row r="40" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3207,17 +3207,17 @@
     <row r="42" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
     </row>
     <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -3233,17 +3233,17 @@
     </row>
     <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3251,7 +3251,7 @@
     </row>
     <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3259,7 +3259,7 @@
     </row>
     <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3267,7 +3267,7 @@
     </row>
     <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3275,7 +3275,7 @@
     </row>
     <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3283,7 +3283,7 @@
     </row>
     <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3291,7 +3291,7 @@
     </row>
     <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3302,12 +3302,12 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3315,7 +3315,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -3323,7 +3323,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3334,10 +3334,10 @@
         <v>92</v>
       </c>
       <c r="B78" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>51</v>
@@ -3348,10 +3348,10 @@
         <v>3501</v>
       </c>
       <c r="B79" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C79" s="22" t="s">
         <v>241</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>242</v>
       </c>
       <c r="D79" s="21">
         <v>33966</v>
@@ -3362,10 +3362,10 @@
         <v>3501005</v>
       </c>
       <c r="B80" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="22" t="s">
         <v>243</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>244</v>
       </c>
       <c r="D80" s="21">
         <v>38477</v>
@@ -3376,10 +3376,10 @@
         <v>3501011</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D81" s="21">
         <v>37964</v>
@@ -3390,10 +3390,10 @@
         <v>3501012</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D82" s="21">
         <v>29667</v>
@@ -3404,10 +3404,10 @@
         <v>3501020</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D83" s="21">
         <v>32716</v>
@@ -3418,10 +3418,10 @@
         <v>3501030</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D84" s="21">
         <v>39345</v>
@@ -3432,10 +3432,10 @@
         <v>3501042</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D85" s="21">
         <v>37020</v>
@@ -3446,10 +3446,10 @@
         <v>3501050</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D86" s="21">
         <v>32181</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,7 +3471,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3479,7 +3479,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3490,10 +3490,10 @@
         <v>92</v>
       </c>
       <c r="B101" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C101" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="C101" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="D101" s="20" t="s">
         <v>157</v>
@@ -3504,10 +3504,10 @@
         <v>3501</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D102" s="21">
         <v>91165</v>
@@ -3518,10 +3518,10 @@
         <v>3501005</v>
       </c>
       <c r="B103" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C103" s="22" t="s">
         <v>243</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>244</v>
       </c>
       <c r="D103" s="21">
         <v>10950</v>
@@ -3532,10 +3532,10 @@
         <v>3501011</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D104" s="21">
         <v>10450</v>
@@ -3546,10 +3546,10 @@
         <v>3501012</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D105" s="21">
         <v>37745</v>
@@ -3560,10 +3560,10 @@
         <v>3501020</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D106" s="21">
         <v>8990</v>
@@ -3574,10 +3574,10 @@
         <v>3501030</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C107" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D107" s="21">
         <v>9255</v>
@@ -3588,10 +3588,10 @@
         <v>3501042</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C108" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D108" s="21">
         <v>5440</v>
@@ -3602,10 +3602,10 @@
         <v>3501050</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C109" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D109" s="21">
         <v>8330</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
@@ -3635,7 +3635,7 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added form instruction as slot field in dhis2 import
</commit_message>
<xml_diff>
--- a/indicators/tests/data/dhis2-indicators.xlsx
+++ b/indicators/tests/data/dhis2-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-20000" windowWidth="31860" windowHeight="19000" tabRatio="841" activeTab="6"/>
+    <workbookView xWindow="160" yWindow="-19840" windowWidth="31860" windowHeight="19000" tabRatio="841"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="268">
   <si>
     <t>Indicator name</t>
   </si>
@@ -966,6 +966,15 @@
   </si>
   <si>
     <t>OptionCode (32 chars max)</t>
+  </si>
+  <si>
+    <t>Form instructions</t>
+  </si>
+  <si>
+    <t>Informational text to appear at the beginning of the form/survey</t>
+  </si>
+  <si>
+    <t>For each statement below, please indicate your level of agreement on a scale from 1 to 5, where 1 means "strongly disagree" and 5 means "strongly agree"</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1129,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1234,6 +1243,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1570,9 +1582,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1604,7 +1616,7 @@
     <col min="24" max="16384" width="17.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1680,8 +1692,11 @@
       <c r="Y1" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.2">
+      <c r="Z1" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1742,8 +1757,11 @@
       <c r="Y2" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="Z2" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="135" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -1795,8 +1813,11 @@
       <c r="W3" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="Z3" s="42" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -1849,7 +1870,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1902,7 +1923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>73</v>
       </c>
@@ -1957,7 +1978,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="28" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="28" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>84</v>
       </c>
@@ -2961,7 +2982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>